<commit_message>
Commit 6: Added NearestNeighbor.py algorithm and supporting methods for delivering packages.
</commit_message>
<xml_diff>
--- a/resource/WGUPS Distance Table.xlsx
+++ b/resource/WGUPS Distance Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mopea\PycharmProjects\C950_Delivery\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940B2E26-9D3B-4DAA-BC3D-B12965A77FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C22DFC-826D-40B1-9AD9-34B29BA6A930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="105" windowWidth="14610" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2535" yWindow="1140" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t xml:space="preserve"> HUB</t>
-  </si>
   <si>
     <t>1330 2100 S</t>
   </si>
@@ -108,6 +105,9 @@
   <si>
     <t>5383 South 900 East #104</t>
   </si>
+  <si>
+    <t>4001 South 700 East</t>
+  </si>
 </sst>
 </file>
 
@@ -116,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,14 +125,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -365,13 +357,13 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -711,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,8 +715,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
+      <c r="A1" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="B1" s="5">
         <v>0</v>
@@ -757,8 +749,8 @@
       <c r="AB1" s="7"/>
     </row>
     <row r="2" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>24</v>
+      <c r="A2" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="B2" s="4">
         <v>7.2</v>
@@ -793,8 +785,8 @@
       <c r="AB2" s="8"/>
     </row>
     <row r="3" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>1</v>
+      <c r="A3" s="12" t="s">
+        <v>0</v>
       </c>
       <c r="B3" s="4">
         <v>3.8</v>
@@ -831,8 +823,8 @@
       <c r="AB3" s="8"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>2</v>
+      <c r="A4" s="12" t="s">
+        <v>1</v>
       </c>
       <c r="B4" s="4">
         <v>11</v>
@@ -871,8 +863,8 @@
       <c r="AB4" s="8"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>3</v>
+      <c r="A5" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="B5" s="4">
         <v>2.2000000000000002</v>
@@ -913,8 +905,8 @@
       <c r="AB5" s="8"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>4</v>
+      <c r="A6" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="B6" s="4">
         <v>3.5</v>
@@ -957,8 +949,8 @@
       <c r="AB6" s="8"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>5</v>
+      <c r="A7" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="B7" s="4">
         <v>10.9</v>
@@ -1003,8 +995,8 @@
       <c r="AB7" s="8"/>
     </row>
     <row r="8" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>6</v>
+      <c r="A8" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="B8" s="4">
         <v>8.6</v>
@@ -1051,8 +1043,8 @@
       <c r="AB8" s="8"/>
     </row>
     <row r="9" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>7</v>
+      <c r="A9" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B9" s="4">
         <v>7.6</v>
@@ -1101,8 +1093,8 @@
       <c r="AB9" s="8"/>
     </row>
     <row r="10" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>8</v>
+      <c r="A10" s="12" t="s">
+        <v>7</v>
       </c>
       <c r="B10" s="4">
         <v>2.8</v>
@@ -1153,8 +1145,8 @@
       <c r="AB10" s="8"/>
     </row>
     <row r="11" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>9</v>
+      <c r="A11" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="B11" s="4">
         <v>6.4</v>
@@ -1207,8 +1199,8 @@
       <c r="AB11" s="8"/>
     </row>
     <row r="12" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>25</v>
+      <c r="A12" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="B12" s="4">
         <v>3.2</v>
@@ -1263,8 +1255,8 @@
       <c r="AB12" s="8"/>
     </row>
     <row r="13" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>10</v>
+      <c r="A13" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="B13" s="4">
         <v>7.6</v>
@@ -1321,8 +1313,8 @@
       <c r="AB13" s="8"/>
     </row>
     <row r="14" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>11</v>
+      <c r="A14" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="B14" s="4">
         <v>5.2</v>
@@ -1381,8 +1373,8 @@
       <c r="AB14" s="8"/>
     </row>
     <row r="15" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>12</v>
+      <c r="A15" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="B15" s="4">
         <v>4.4000000000000004</v>
@@ -1443,8 +1435,8 @@
       <c r="AB15" s="8"/>
     </row>
     <row r="16" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>13</v>
+      <c r="A16" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="B16" s="4">
         <v>3.66112816434</v>
@@ -1507,8 +1499,8 @@
       <c r="AB16" s="8"/>
     </row>
     <row r="17" spans="1:28" ht="36" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>14</v>
+      <c r="A17" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="B17" s="4">
         <v>7.6</v>
@@ -1573,8 +1565,8 @@
       <c r="AB17" s="8"/>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>15</v>
+      <c r="A18" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="B18" s="4">
         <v>2</v>
@@ -1641,8 +1633,8 @@
       <c r="AB18" s="8"/>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>16</v>
+      <c r="A19" s="12" t="s">
+        <v>15</v>
       </c>
       <c r="B19" s="4">
         <v>3.6</v>
@@ -1711,8 +1703,8 @@
       <c r="AB19" s="8"/>
     </row>
     <row r="20" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>17</v>
+      <c r="A20" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="B20" s="4">
         <v>6.5</v>
@@ -1783,8 +1775,8 @@
       <c r="AB20" s="8"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>18</v>
+      <c r="A21" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="B21" s="4">
         <v>1.9</v>
@@ -1857,8 +1849,8 @@
       <c r="AB21" s="8"/>
     </row>
     <row r="22" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>19</v>
+      <c r="A22" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="B22" s="4">
         <v>3.4</v>
@@ -1933,8 +1925,8 @@
       <c r="AB22" s="8"/>
     </row>
     <row r="23" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>20</v>
+      <c r="A23" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="B23" s="4">
         <v>2.4</v>
@@ -2011,8 +2003,8 @@
       <c r="AB23" s="8"/>
     </row>
     <row r="24" spans="1:28" ht="24" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>21</v>
+      <c r="A24" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="B24" s="4">
         <v>6.4</v>
@@ -2091,8 +2083,8 @@
       <c r="AB24" s="8"/>
     </row>
     <row r="25" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>26</v>
+      <c r="A25" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="B25" s="4">
         <v>2.4</v>
@@ -2173,8 +2165,8 @@
       <c r="AB25" s="8"/>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>22</v>
+      <c r="A26" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="B26" s="4">
         <v>5</v>
@@ -2257,8 +2249,8 @@
       <c r="AB26" s="8"/>
     </row>
     <row r="27" spans="1:28" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
-        <v>23</v>
+      <c r="A27" s="13" t="s">
+        <v>22</v>
       </c>
       <c r="B27" s="9">
         <v>3.6</v>

</xml_diff>